<commit_message>
update export format template
</commit_message>
<xml_diff>
--- a/banking-report-service/src/main/resources/template/excel/account.xlsx
+++ b/banking-report-service/src/main/resources/template/excel/account.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nvs/Downloads/Work/KLB/microservices-core-banking/banking-report-service/src/main/resources/template/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E118266E-0B27-A94C-82BC-E1108BF61682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8446A1DA-D8F9-4F4F-A5AA-6A3BFAB5EEF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{E2CCA71D-B452-3C4E-A0F0-45F48612AB07}"/>
   </bookViews>
@@ -266,9 +266,6 @@
     <t>${account.status}</t>
   </si>
   <si>
-    <t>${account.id}</t>
-  </si>
-  <si>
     <t>${account.availableBalance}</t>
   </si>
   <si>
@@ -276,6 +273,9 @@
   </si>
   <si>
     <t>Số dư khả dụng (Balance)</t>
+  </si>
+  <si>
+    <t>${account.no}</t>
   </si>
 </sst>
 </file>
@@ -503,6 +503,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -536,8 +538,6 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -855,7 +855,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -872,140 +872,140 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="13"/>
     </row>
     <row r="2" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="9"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="11"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="13"/>
     </row>
     <row r="3" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="12"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="14"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="16"/>
     </row>
     <row r="7" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="5"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="7"/>
     </row>
     <row r="9" spans="1:7" ht="20" x14ac:dyDescent="0.2">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="15" t="s">
+      <c r="G9" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="20" x14ac:dyDescent="0.2">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="16" t="s">
+      <c r="B10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="F10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="G10" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="8"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="10"/>
       <c r="G15" s="3"/>
     </row>
     <row r="17" spans="1:7" ht="20" x14ac:dyDescent="0.2">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D17" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="F17" s="15" t="s">
+      <c r="E17" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" s="4" t="s">
         <v>20</v>
       </c>
       <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="E18" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="F18" s="16" t="s">
+      <c r="F18" s="5" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
refactor response with resource for file format
</commit_message>
<xml_diff>
--- a/banking-report-service/src/main/resources/template/excel/account.xlsx
+++ b/banking-report-service/src/main/resources/template/excel/account.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nvs/Downloads/Work/KLB/microservices-core-banking/banking-report-service/src/main/resources/template/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8446A1DA-D8F9-4F4F-A5AA-6A3BFAB5EEF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A70C0A2-3231-4C4B-8CFC-04B5C2D0F331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{E2CCA71D-B452-3C4E-A0F0-45F48612AB07}"/>
+    <workbookView xWindow="0" yWindow="640" windowWidth="29400" windowHeight="18480" xr2:uid="{E2CCA71D-B452-3C4E-A0F0-45F48612AB07}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -68,10 +68,8 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">jx:mergeCells(cols="7" rows="3" minCols="A1" minRows="A1" lastCell="G3") 
-</t>
+          </rPr>
+          <t>jx:mergeCells(lastCell="G3" cols="7" rows="3" minCols="A1" minRows="A1")</t>
         </r>
       </text>
     </comment>
@@ -282,7 +280,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -316,32 +314,47 @@
       <family val="1"/>
     </font>
     <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
       <sz val="36"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
     <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
       <sz val="16"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -498,44 +511,57 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -852,13 +878,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B9E8742-DA2D-6D4A-BF79-AE3C8E7A31A7}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="39.1640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="40.5" style="1" customWidth="1"/>
@@ -871,145 +897,152 @@
     <col min="9" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="13"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="7"/>
     </row>
-    <row r="2" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="11"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="13"/>
+    <row r="2" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="7"/>
     </row>
-    <row r="3" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="14"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="16"/>
+    <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="8"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="10"/>
     </row>
-    <row r="7" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="7"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="12"/>
     </row>
-    <row r="9" spans="1:7" ht="20" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="20" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
+    <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+    <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="10"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="17"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="17" spans="1:7" ht="20" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
+    <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="14"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+    </row>
+    <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="G17" s="2"/>
+      <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
+    <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="F18" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A7:G7"/>

</xml_diff>

<commit_message>
pull main and fix Override
</commit_message>
<xml_diff>
--- a/banking-report-service/src/main/resources/template/excel/account.xlsx
+++ b/banking-report-service/src/main/resources/template/excel/account.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nvs/Downloads/Work/KLB/microservices-core-banking/banking-report-service/src/main/resources/template/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A70C0A2-3231-4C4B-8CFC-04B5C2D0F331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20CEA7E-CB36-2145-B2A2-1FE59F73B1F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="640" windowWidth="29400" windowHeight="18480" xr2:uid="{E2CCA71D-B452-3C4E-A0F0-45F48612AB07}"/>
   </bookViews>
@@ -40,15 +40,16 @@
     <author>Nguyễn Văn Sĩ</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{0F6EBF93-FBFE-7245-AD5C-FC94FB3A4C21}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{5345B9F4-D818-8848-B82E-2CCD604BC9B5}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
           </rPr>
           <t>Nguyễn Văn Sĩ:</t>
         </r>
@@ -56,8 +57,9 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -68,8 +70,45 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
+            <scheme val="minor"/>
           </rPr>
           <t>jx:mergeCells(lastCell="G3" cols="7" rows="3" minCols="A1" minRows="A1")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{DB5ABC8E-783D-0148-BD41-229D5A7EF353}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Nguyễn Văn Sĩ:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>jx:area(lastCell="B5")</t>
         </r>
       </text>
     </comment>
@@ -187,7 +226,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Báo cáo tài khoản</t>
   </si>
@@ -274,13 +313,19 @@
   </si>
   <si>
     <t>${account.no}</t>
+  </si>
+  <si>
+    <t>Ngày báo cáo:</t>
+  </si>
+  <si>
+    <t>${reportDate}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -358,6 +403,36 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -511,7 +586,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -525,6 +600,27 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -543,26 +639,8 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -579,6 +657,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -881,7 +963,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -898,65 +980,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="7"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="14"/>
     </row>
     <row r="2" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="5"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="7"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="14"/>
     </row>
     <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="8"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="10"/>
+      <c r="A3" s="15"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="17"/>
+    </row>
+    <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="12"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="8"/>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="G9" s="5" t="s">
         <v>15</v>
       </c>
     </row>
@@ -984,41 +1074,41 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="17"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="11"/>
       <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="14"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
     </row>
     <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="E17" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F17" s="13" t="s">
+      <c r="F17" s="5" t="s">
         <v>20</v>
       </c>
       <c r="G17" s="4"/>

</xml_diff>